<commit_message>
correct erroneous context words on animal sheet, with new dwnload from English Corpora
</commit_message>
<xml_diff>
--- a/practicals/contexts.xlsx
+++ b/practicals/contexts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/vc/nlp_youth_awards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angus/vc/nlp-half-day-workshop/practicals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DEF66F-7AA9-3549-9548-C28D318983A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717D07AF-7305-AC4C-93B2-56BB776F473E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="2900" windowWidth="25560" windowHeight="14620" activeTab="8" xr2:uid="{93BF21BB-41B4-D544-8F23-BCC3D9D3D76D}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="291">
   <si>
     <t>salad</t>
   </si>
@@ -820,158 +820,110 @@
     <t>cat</t>
   </si>
   <si>
-    <t>pecies</t>
-  </si>
-  <si>
-    <t>ildlife</t>
-  </si>
-  <si>
-    <t>nimal</t>
-  </si>
-  <si>
-    <t>gg</t>
-  </si>
-  <si>
-    <t>ree</t>
-  </si>
-  <si>
-    <t>est</t>
-  </si>
-  <si>
-    <t>abitat</t>
-  </si>
-  <si>
-    <t>eed</t>
-  </si>
-  <si>
-    <t>orest</t>
-  </si>
-  <si>
-    <t>ild</t>
-  </si>
-  <si>
-    <t>eather</t>
-  </si>
-  <si>
-    <t>ly</t>
-  </si>
-  <si>
-    <t>sland</t>
-  </si>
-  <si>
-    <t>ing</t>
-  </si>
-  <si>
-    <t>arden</t>
-  </si>
-  <si>
-    <t>lant</t>
-  </si>
-  <si>
-    <t>ark</t>
-  </si>
-  <si>
-    <t>hicken</t>
-  </si>
-  <si>
-    <t>nsect</t>
-  </si>
-  <si>
-    <t>ish</t>
-  </si>
-  <si>
-    <t>inter</t>
-  </si>
-  <si>
-    <t>reeding</t>
-  </si>
-  <si>
-    <t>iver</t>
-  </si>
-  <si>
-    <t>opulation</t>
-  </si>
-  <si>
-    <t>ea</t>
-  </si>
-  <si>
-    <t>ake</t>
-  </si>
-  <si>
-    <t>rey</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>emale</t>
-  </si>
-  <si>
-    <t>ale</t>
-  </si>
-  <si>
-    <t>each</t>
-  </si>
-  <si>
-    <t>ammal</t>
-  </si>
-  <si>
-    <t>uman</t>
-  </si>
-  <si>
-    <t>ature</t>
-  </si>
-  <si>
-    <t>ative</t>
-  </si>
-  <si>
-    <t>lock</t>
-  </si>
-  <si>
-    <t>ail</t>
-  </si>
-  <si>
-    <t>redator</t>
-  </si>
-  <si>
-    <t>ountain</t>
-  </si>
-  <si>
-    <t>reature</t>
-  </si>
-  <si>
-    <t>arm</t>
-  </si>
-  <si>
-    <t>unting</t>
-  </si>
-  <si>
-    <t>light</t>
-  </si>
-  <si>
-    <t>et</t>
-  </si>
-  <si>
-    <t>uck</t>
-  </si>
-  <si>
-    <t>agle</t>
-  </si>
-  <si>
-    <t>pring</t>
-  </si>
-  <si>
-    <t>rail</t>
-  </si>
-  <si>
-    <t>at</t>
+    <t>welfare</t>
+  </si>
+  <si>
+    <t>care</t>
+  </si>
+  <si>
+    <t>shelter</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>cruelty</t>
+  </si>
+  <si>
+    <t>kingdom</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>behavior</t>
+  </si>
+  <si>
+    <t>companion</t>
+  </si>
+  <si>
+    <t>zoo</t>
+  </si>
+  <si>
+    <t>rescue</t>
+  </si>
+  <si>
+    <t>lover</t>
+  </si>
+  <si>
+    <t>hospital</t>
+  </si>
+  <si>
+    <t>spirit</t>
+  </si>
+  <si>
+    <t>laboratory</t>
+  </si>
+  <si>
+    <t>planet</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>abuse</t>
+  </si>
+  <si>
+    <t>horse</t>
+  </si>
+  <si>
+    <t>print</t>
+  </si>
+  <si>
+    <t>bone</t>
+  </si>
+  <si>
+    <t>activist</t>
+  </si>
+  <si>
+    <t>husbandry</t>
+  </si>
+  <si>
+    <t>experiment</t>
+  </si>
+  <si>
+    <t>being</t>
+  </si>
+  <si>
+    <t>tissue</t>
+  </si>
+  <si>
+    <t>sacrifice</t>
+  </si>
+  <si>
+    <t>waste</t>
+  </si>
+  <si>
+    <t>sanctuary</t>
+  </si>
+  <si>
+    <t>adoption</t>
+  </si>
+  <si>
+    <t>agriculture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1000,6 +952,12 @@
       <color rgb="FF000000"/>
       <name val="Aptos"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1027,7 +985,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1047,6 +1005,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1383,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E46DB57-D1BD-3E4B-AD37-0B653023E1A8}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2016,7 +1989,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5903,7 +5876,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6534,14 +6507,14 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -6551,608 +6524,608 @@
       <c r="B1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>35658</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C2" s="4">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>64067</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="12">
         <f>ROUND(((A2/$A$2)*100),0)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>30991</v>
-      </c>
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>36534</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="12">
+        <f t="shared" ref="C3:C51" si="0">ROUND(((A3/$A$2)*100),0)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>32169</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="12">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>25677</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="C3" s="4">
-        <f t="shared" ref="C3:C51" si="0">ROUND(((A3/$A$2)*100),0)</f>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>30084</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="12">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>24900</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>22929</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="C4" s="4">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>23651</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C7" s="12">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>22163</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>20867</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C5" s="4">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>23419</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C9" s="12">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>20134</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C6" s="4">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>17882</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C10" s="12">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>17976</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="C7" s="4">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>17171</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C11" s="12">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>17554</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="C8" s="4">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>16162</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C12" s="12">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>16459</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="C9" s="4">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>14778</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C13" s="12">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>14948</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="C10" s="4">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>14625</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="C14" s="12">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>14183</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>12205</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="C11" s="4">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>14463</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="C16" s="12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>11577</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="C12" s="4">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>14242</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C17" s="12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>11532</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="C13" s="4">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>13396</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="C18" s="12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>11300</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="12">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>11189</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="C14" s="4">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
-        <v>12668</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="C20" s="12">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>10565</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="C15" s="4">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
-        <v>12404</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="C21" s="12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>8970</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="C16" s="4">
-        <f t="shared" si="0"/>
+      <c r="C22" s="12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>8931</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>8784</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C24" s="12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>8300</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="12">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>7935</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C26" s="12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>6891</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C27" s="12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>6887</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="C28" s="12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>6773</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="C29" s="12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>6196</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="C30" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>6177</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C31" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>6025</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="C32" s="12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>5641</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C33" s="12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>5635</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="C34" s="12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>5184</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C35" s="12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>5137</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="C36" s="12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>4877</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C37" s="12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
+        <v>4572</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="C38" s="12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>4544</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
+        <v>4056</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C40" s="12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
+        <v>3975</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C41" s="12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>3851</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C42" s="12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>3827</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="C43" s="12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>3750</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="C44" s="12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>3636</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C45" s="12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="9">
+        <v>3580</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C46" s="12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>3523</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C47" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
+        <v>3474</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C48" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>3428</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C49" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>3254</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>12191</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="C17" s="4">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>12029</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C18" s="4">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>11850</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="C19" s="4">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
-        <v>11808</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C20" s="4">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>11537</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C21" s="4">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
-        <v>11422</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="C22" s="4">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="5">
-        <v>10950</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="C23" s="4">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
-        <v>10865</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="5">
-        <v>10690</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="C25" s="4">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
-        <v>10143</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="C26" s="4">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="5">
-        <v>9749</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C27" s="4">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="5">
-        <v>9729</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="C28" s="4">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5">
-        <v>9604</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="C29" s="4">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="5">
-        <v>9510</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C30" s="4">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="5">
-        <v>9426</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="C31" s="4">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
-        <v>9326</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C32" s="4">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="5">
-        <v>9255</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="C33" s="4">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
-        <v>9203</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="C34" s="4">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
-        <v>9143</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="C35" s="4">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
-        <v>8411</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C36" s="4">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
-        <v>8389</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C37" s="4">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
-        <v>8274</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="C38" s="4">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
-        <v>8233</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="C39" s="4">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
-        <v>8228</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C40" s="4">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
-        <v>8183</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="C41" s="4">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
-        <v>8118</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C42" s="4">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
-        <v>8057</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="C43" s="4">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="5">
-        <v>7998</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="C44" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="5">
-        <v>7929</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="C45" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
-        <v>7910</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="C46" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="5">
-        <v>7857</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="C47" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="5">
-        <v>7822</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="C48" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="5">
-        <v>7667</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="C49" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="5">
-        <v>7648</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="C50" s="4">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="5">
-        <v>7638</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C51" s="4">
-        <f t="shared" si="0"/>
-        <v>21</v>
+      <c r="C50" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="9">
+        <v>3193</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C51" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>